<commit_message>
Need final data dictionary from Scott
</commit_message>
<xml_diff>
--- a/SideProjects/CityOfToronto_Tools/GraphicsReportAutomation_QCQA/Data/MasterOutputs/2022-02-10_QC_MasterFile_Etobicoke York District.xlsx
+++ b/SideProjects/CityOfToronto_Tools/GraphicsReportAutomation_QCQA/Data/MasterOutputs/2022-02-10_QC_MasterFile_Etobicoke York District.xlsx
@@ -789,6 +789,14 @@
       <formula>-99999999999</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
+      <formula1>"Not Checked,In Progress,Checked"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H11">
+      <formula1>"Scott,Roger,Rudy,Ren"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>